<commit_message>
some chnages to renaming the Hnf files
</commit_message>
<xml_diff>
--- a/masters/autodownlaod_mail.xlsx
+++ b/masters/autodownlaod_mail.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>Hotel_name</t>
   </si>
@@ -56,15 +56,21 @@
   </si>
   <si>
     <t>HNF_HotelCentrePoint.xlsx</t>
+  </si>
+  <si>
+    <t>2022-06-21 09:30:54</t>
+  </si>
+  <si>
+    <t>2022-06-17 11:00:06</t>
+  </si>
+  <si>
+    <t>2022-06-19 12:00:08</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="YYYY-MM-DD HH:MM:SS"/>
-  </numFmts>
   <fonts count="2">
     <font>
       <sz val="11"/>
@@ -117,12 +123,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -453,8 +458,8 @@
       <c r="D2">
         <v>1</v>
       </c>
-      <c r="E2" s="2">
-        <v>44693.45022686834</v>
+      <c r="E2" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -470,8 +475,8 @@
       <c r="D3">
         <v>0</v>
       </c>
-      <c r="E3">
-        <v>1.652272007939e+18</v>
+      <c r="E3" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -485,10 +490,10 @@
         <v>13</v>
       </c>
       <c r="D4">
-        <v>1</v>
-      </c>
-      <c r="E4" s="2">
-        <v>44693.45025361342</v>
+        <v>0</v>
+      </c>
+      <c r="E4" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>